<commit_message>
Decorado y con repsonsabilidades.
</commit_message>
<xml_diff>
--- a/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosFormulario.xlsx
+++ b/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosFormulario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="38">
   <si>
     <t>Periodo</t>
   </si>
@@ -138,21 +138,6 @@
   </si>
   <si>
     <t>fghdgsd</t>
-  </si>
-  <si>
-    <t>2014098673</t>
-  </si>
-  <si>
-    <t>Erick1</t>
-  </si>
-  <si>
-    <t>erick.hdez06@outlook.com</t>
-  </si>
-  <si>
-    <t>22222222</t>
-  </si>
-  <si>
-    <t>Oh no!!!</t>
   </si>
 </sst>
 </file>
@@ -200,10 +185,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -687,7 +694,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="133">
+      <c r="A2" t="n" s="157">
         <v>42789.0</v>
       </c>
       <c r="B2" t="s">
@@ -726,7 +733,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="135">
+      <c r="A3" t="n" s="159">
         <v>42825.0</v>
       </c>
       <c r="B3" t="s">
@@ -765,7 +772,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="137">
+      <c r="A4" t="n" s="161">
         <v>43285.95474537037</v>
       </c>
       <c r="B4" t="s">
@@ -802,45 +809,6 @@
         <v>37</v>
       </c>
       <c r="M4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n" s="139">
-        <v>42902.86296784722</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I5"/>
-      <c r="J5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
creo que ya arregle ese bug del que no carga resoluciones
</commit_message>
<xml_diff>
--- a/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosFormulario.xlsx
+++ b/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosFormulario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="49">
   <si>
     <t>Periodo</t>
   </si>
@@ -138,6 +138,39 @@
   </si>
   <si>
     <t>fghdgsd</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>pato</t>
+  </si>
+  <si>
+    <t>pato@gmail.com</t>
+  </si>
+  <si>
+    <t>60990312</t>
+  </si>
+  <si>
+    <t>IC1802</t>
+  </si>
+  <si>
+    <t>MODIFICACIÓN_ACTA</t>
+  </si>
+  <si>
+    <t>prueba</t>
+  </si>
+  <si>
+    <t>patito</t>
+  </si>
+  <si>
+    <t>b@g.com</t>
+  </si>
+  <si>
+    <t>20998766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:V </t>
   </si>
 </sst>
 </file>
@@ -185,10 +218,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -694,7 +745,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="157">
+      <c r="A2" t="n" s="171">
         <v>42789.0</v>
       </c>
       <c r="B2" t="s">
@@ -733,7 +784,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="159">
+      <c r="A3" t="n" s="173">
         <v>42825.0</v>
       </c>
       <c r="B3" t="s">
@@ -772,7 +823,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="161">
+      <c r="A4" t="n" s="175">
         <v>43285.95474537037</v>
       </c>
       <c r="B4" t="s">
@@ -809,6 +860,88 @@
         <v>37</v>
       </c>
       <c r="M4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="177">
+        <v>42903.51540038195</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="179">
+        <v>42903.51825075231</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ya mejores macros y un poco pegado lo de los templates
</commit_message>
<xml_diff>
--- a/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosFormulario.xlsx
+++ b/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosFormulario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="38">
   <si>
     <t>Periodo</t>
   </si>
@@ -138,39 +138,6 @@
   </si>
   <si>
     <t>fghdgsd</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>pato</t>
-  </si>
-  <si>
-    <t>pato@gmail.com</t>
-  </si>
-  <si>
-    <t>60990312</t>
-  </si>
-  <si>
-    <t>IC1802</t>
-  </si>
-  <si>
-    <t>MODIFICACIÓN_ACTA</t>
-  </si>
-  <si>
-    <t>prueba</t>
-  </si>
-  <si>
-    <t>patito</t>
-  </si>
-  <si>
-    <t>b@g.com</t>
-  </si>
-  <si>
-    <t>20998766</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:V </t>
   </si>
 </sst>
 </file>
@@ -218,58 +185,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -745,7 +664,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="171">
+      <c r="A2" t="n" s="127">
         <v>42789.0</v>
       </c>
       <c r="B2" t="s">
@@ -784,7 +703,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="173">
+      <c r="A3" t="n" s="129">
         <v>42825.0</v>
       </c>
       <c r="B3" t="s">
@@ -823,7 +742,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="175">
+      <c r="A4" t="n" s="131">
         <v>43285.95474537037</v>
       </c>
       <c r="B4" t="s">
@@ -860,88 +779,6 @@
         <v>37</v>
       </c>
       <c r="M4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n" s="177">
-        <v>42903.51540038195</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I5" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n" s="179">
-        <v>42903.51825075231</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" t="s">
-        <v>45</v>
-      </c>
-      <c r="M6" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ya no se altera el tamano
</commit_message>
<xml_diff>
--- a/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosFormulario.xlsx
+++ b/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosFormulario.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -125,15 +125,97 @@
   </si>
   <si>
     <t xml:space="preserve">fghdgsd</t>
+  </si>
+  <si>
+    <t>Id solicitante</t>
+  </si>
+  <si>
+    <t>Nombre solicitante</t>
+  </si>
+  <si>
+    <t>Estado de solicitud</t>
+  </si>
+  <si>
+    <t>Num de Resolucion</t>
+  </si>
+  <si>
+    <t>2011123456</t>
+  </si>
+  <si>
+    <t>Estudiante 1</t>
+  </si>
+  <si>
+    <t>xbolanosfonseca@gmail.com</t>
+  </si>
+  <si>
+    <t>89999999</t>
+  </si>
+  <si>
+    <t>IS2017</t>
+  </si>
+  <si>
+    <t>IC4301</t>
+  </si>
+  <si>
+    <t>ERROR_NOTA</t>
+  </si>
+  <si>
+    <t>Me pusieron un 65 cuando lo correcto era un 75</t>
+  </si>
+  <si>
+    <t>PENDIENTE</t>
+  </si>
+  <si>
+    <t>2015567890</t>
+  </si>
+  <si>
+    <t>Estudiante 2</t>
+  </si>
+  <si>
+    <t>59999999</t>
+  </si>
+  <si>
+    <t>IC5821</t>
+  </si>
+  <si>
+    <t>Me pusieron un 70 cuando lo correcto era un 75, porque al final de me dio un 72.51</t>
+  </si>
+  <si>
+    <t>PROCESADA</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>21345</t>
+  </si>
+  <si>
+    <t>fgdfg</t>
+  </si>
+  <si>
+    <t>8888-8888</t>
+  </si>
+  <si>
+    <t>EXCLUSION_ACTA</t>
+  </si>
+  <si>
+    <t>2453534</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>fghdgsd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D/M/YY"/>
+    <numFmt numFmtId="166" formatCode="d/m/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -209,7 +291,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -222,6 +304,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -247,17 +335,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.21457489878543"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.57085020242915"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="67.914979757085"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.6032388663968"/>
+    <col min="1" max="1" hidden="false" style="0" width="9.21052631578947" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="10.8178137651822" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="18.6396761133603" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="11.3562753036437" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="6.74898785425101" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="6.21457489878543" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="5.57085020242915" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="11.6761133603239" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="0" width="67.914979757085" collapsed="true"/>
+    <col min="11" max="1025" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -291,128 +379,135 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>13</v>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>42789</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>22</v>
+    <row r="2">
+      <c r="A2" t="n" s="3">
+        <v>42789.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>42825</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>22</v>
+    <row r="3">
+      <c r="A3" t="n" s="5">
+        <v>42825.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>43285.9547453704</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>22</v>
+    <row r="4">
+      <c r="A4" t="n" s="7">
+        <v>43285.95474537037</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios en la interfaz para bien
</commit_message>
<xml_diff>
--- a/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosFormulario.xlsx
+++ b/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosFormulario.xlsx
@@ -184,7 +184,7 @@
     <t>PROCESADA</t>
   </si>
   <si>
-    <t>17</t>
+    <t>24</t>
   </si>
   <si>
     <t>21345</t>
@@ -329,8 +329,8 @@
   </sheetPr>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D2:D4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N2:N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -338,13 +338,13 @@
     <col min="1" max="1" hidden="false" style="0" width="9.21052631578947" collapsed="true"/>
     <col min="2" max="2" hidden="false" style="0" width="10.8178137651822" collapsed="true"/>
     <col min="3" max="3" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="18.6396761133603" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="18.7449392712551" collapsed="true"/>
     <col min="5" max="5" hidden="false" style="0" width="11.3562753036437" collapsed="true"/>
     <col min="6" max="6" hidden="false" style="0" width="6.74898785425101" collapsed="true"/>
     <col min="7" max="7" hidden="false" style="0" width="6.21457489878543" collapsed="true"/>
     <col min="8" max="8" hidden="false" style="0" width="5.57085020242915" collapsed="true"/>
     <col min="9" max="9" hidden="false" style="0" width="11.6761133603239" collapsed="true"/>
-    <col min="10" max="10" hidden="false" style="0" width="67.914979757085" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="0" width="68.4493927125506" collapsed="true"/>
     <col min="11" max="1025" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Ya muestra la resolución en la web
</commit_message>
<xml_diff>
--- a/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosFormulario.xlsx
+++ b/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosFormulario.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -125,15 +125,97 @@
   </si>
   <si>
     <t xml:space="preserve">fghdgsd</t>
+  </si>
+  <si>
+    <t>Id solicitante</t>
+  </si>
+  <si>
+    <t>Nombre solicitante</t>
+  </si>
+  <si>
+    <t>Estado de solicitud</t>
+  </si>
+  <si>
+    <t>Num de Resolucion</t>
+  </si>
+  <si>
+    <t>2011123456</t>
+  </si>
+  <si>
+    <t>Estudiante 1</t>
+  </si>
+  <si>
+    <t>xbolanosfonseca@gmail.com</t>
+  </si>
+  <si>
+    <t>89999999</t>
+  </si>
+  <si>
+    <t>IS2017</t>
+  </si>
+  <si>
+    <t>IC4301</t>
+  </si>
+  <si>
+    <t>ERROR_NOTA</t>
+  </si>
+  <si>
+    <t>Me pusieron un 65 cuando lo correcto era un 75</t>
+  </si>
+  <si>
+    <t>PENDIENTE</t>
+  </si>
+  <si>
+    <t>2015567890</t>
+  </si>
+  <si>
+    <t>Estudiante 2</t>
+  </si>
+  <si>
+    <t>59999999</t>
+  </si>
+  <si>
+    <t>IC5821</t>
+  </si>
+  <si>
+    <t>Me pusieron un 70 cuando lo correcto era un 75, porque al final de me dio un 72.51</t>
+  </si>
+  <si>
+    <t>PROCESADA</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>21345</t>
+  </si>
+  <si>
+    <t>fgdfg</t>
+  </si>
+  <si>
+    <t>8888-8888</t>
+  </si>
+  <si>
+    <t>EXCLUSION_ACTA</t>
+  </si>
+  <si>
+    <t>2453534</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>fghdgsd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D/M/YY"/>
+    <numFmt numFmtId="166" formatCode="d/m/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -209,7 +291,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -222,6 +304,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -247,17 +335,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.21457489878543"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.57085020242915"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="67.914979757085"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.6032388663968"/>
+    <col min="1" max="1" hidden="false" style="0" width="9.21052631578947" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="10.8178137651822" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="18.6396761133603" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="11.3562753036437" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="6.74898785425101" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="6.21457489878543" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="5.57085020242915" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="11.6761133603239" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="0" width="67.914979757085" collapsed="true"/>
+    <col min="11" max="1025" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -291,128 +379,135 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>13</v>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>42789</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>22</v>
+    <row r="2">
+      <c r="A2" t="n" s="3">
+        <v>42789.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>42825</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>22</v>
+    <row r="3">
+      <c r="A3" t="n" s="5">
+        <v>42825.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>43285.9547453704</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>22</v>
+    <row r="4">
+      <c r="A4" t="n" s="7">
+        <v>43285.95474537037</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>